<commit_message>
shuffle practice math round 2
</commit_message>
<xml_diff>
--- a/wmTask/practiceOperations2.xlsx
+++ b/wmTask/practiceOperations2.xlsx
@@ -441,7 +441,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,35 +459,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -503,13 +503,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -547,13 +547,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -580,35 +580,35 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>